<commit_message>
fix rest days for 12hr and 8hr weekday drivers
</commit_message>
<xml_diff>
--- a/5 semester/Driver_Schedule_GA.xlsx
+++ b/5 semester/Driver_Schedule_GA.xlsx
@@ -512,34 +512,34 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>Driver_10_12hr</t>
+          <t>Driver_1_12hr</t>
         </is>
       </c>
       <c r="B3" s="4" t="inlineStr"/>
-      <c r="C3" s="4" t="inlineStr"/>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>14:00 - 02:00</t>
+        </is>
+      </c>
       <c r="D3" s="4" t="inlineStr"/>
       <c r="E3" s="4" t="inlineStr"/>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>14:00 - 02:00</t>
-        </is>
-      </c>
+      <c r="F3" s="4" t="inlineStr"/>
       <c r="G3" s="4" t="inlineStr"/>
       <c r="H3" s="4" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>Driver_11_8hr</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>06:00 - 14:00</t>
-        </is>
-      </c>
+          <t>Driver_8_12hr</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr"/>
       <c r="C4" s="4" t="inlineStr"/>
-      <c r="D4" s="4" t="inlineStr"/>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>14:00 - 02:00</t>
+        </is>
+      </c>
       <c r="E4" s="4" t="inlineStr"/>
       <c r="F4" s="4" t="inlineStr"/>
       <c r="G4" s="4" t="inlineStr"/>
@@ -548,35 +548,35 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Driver_17_12hr</t>
+          <t>Driver_9_12hr</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr"/>
       <c r="C5" s="4" t="inlineStr"/>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr"/>
+      <c r="E5" s="4" t="inlineStr"/>
+      <c r="F5" s="4" t="inlineStr">
         <is>
           <t>14:00 - 02:00</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr"/>
-      <c r="F5" s="4" t="inlineStr"/>
       <c r="G5" s="4" t="inlineStr"/>
       <c r="H5" s="4" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Driver_18_8hr</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr"/>
+          <t>Driver_23_12hr</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>14:00 - 02:00</t>
+        </is>
+      </c>
       <c r="C6" s="4" t="inlineStr"/>
       <c r="D6" s="4" t="inlineStr"/>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>06:00 - 14:00</t>
-        </is>
-      </c>
+      <c r="E6" s="4" t="inlineStr"/>
       <c r="F6" s="4" t="inlineStr"/>
       <c r="G6" s="4" t="inlineStr"/>
       <c r="H6" s="4" t="inlineStr"/>
@@ -584,51 +584,55 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Driver_23_12hr</t>
+          <t>Driver_28_12hr_wk</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr"/>
       <c r="C7" s="4" t="inlineStr"/>
       <c r="D7" s="4" t="inlineStr"/>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>14:00 - 02:00</t>
-        </is>
-      </c>
+      <c r="E7" s="4" t="inlineStr"/>
       <c r="F7" s="4" t="inlineStr"/>
       <c r="G7" s="4" t="inlineStr"/>
-      <c r="H7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>06:00 - 18:00</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Driver_28_12hr_wk</t>
+          <t>Driver_32_8hr</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr"/>
       <c r="C8" s="4" t="inlineStr"/>
-      <c r="D8" s="4" t="inlineStr"/>
-      <c r="E8" s="4" t="inlineStr"/>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>06:00 - 14:00</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>06:00 - 14:00</t>
+        </is>
+      </c>
       <c r="F8" s="4" t="inlineStr"/>
       <c r="G8" s="4" t="inlineStr"/>
-      <c r="H8" s="4" t="inlineStr">
-        <is>
-          <t>06:00 - 18:00</t>
-        </is>
-      </c>
+      <c r="H8" s="4" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Driver_31_12hr</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr"/>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>14:00 - 02:00</t>
-        </is>
-      </c>
+          <t>Driver_33_8hr</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>06:00 - 14:00</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr"/>
       <c r="D9" s="4" t="inlineStr"/>
       <c r="E9" s="4" t="inlineStr"/>
       <c r="F9" s="4" t="inlineStr"/>
@@ -638,35 +642,35 @@
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>Driver_34_12hr_wk</t>
+          <t>Driver_39_8hr</t>
         </is>
       </c>
       <c r="B10" s="4" t="inlineStr"/>
-      <c r="C10" s="4" t="inlineStr"/>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>06:00 - 14:00</t>
+        </is>
+      </c>
       <c r="D10" s="4" t="inlineStr"/>
       <c r="E10" s="4" t="inlineStr"/>
       <c r="F10" s="4" t="inlineStr"/>
-      <c r="G10" s="4" t="inlineStr">
-        <is>
-          <t>06:00 - 18:00</t>
-        </is>
-      </c>
+      <c r="G10" s="4" t="inlineStr"/>
       <c r="H10" s="4" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>Driver_39_8hr</t>
+          <t>Driver_43_12hr</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr"/>
       <c r="C11" s="4" t="inlineStr"/>
-      <c r="D11" s="4" t="inlineStr">
-        <is>
-          <t>06:00 - 14:00</t>
-        </is>
-      </c>
-      <c r="E11" s="4" t="inlineStr"/>
+      <c r="D11" s="4" t="inlineStr"/>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>14:00 - 02:00</t>
+        </is>
+      </c>
       <c r="F11" s="4" t="inlineStr"/>
       <c r="G11" s="4" t="inlineStr"/>
       <c r="H11" s="4" t="inlineStr"/>
@@ -674,7 +678,7 @@
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>Driver_46_8hr</t>
+          <t>Driver_53_8hr</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr"/>
@@ -692,67 +696,67 @@
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Driver_51_12hr</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>14:00 - 02:00</t>
-        </is>
-      </c>
+          <t>Driver_55_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr"/>
       <c r="C13" s="4" t="inlineStr"/>
       <c r="D13" s="4" t="inlineStr"/>
       <c r="E13" s="4" t="inlineStr"/>
       <c r="F13" s="4" t="inlineStr"/>
-      <c r="G13" s="4" t="inlineStr"/>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>06:00 - 18:00</t>
+        </is>
+      </c>
       <c r="H13" s="4" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>Driver_54_8hr</t>
-        </is>
-      </c>
-      <c r="B14" s="4" t="inlineStr"/>
-      <c r="C14" s="4" t="inlineStr">
-        <is>
-          <t>06:00 - 14:00</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="inlineStr"/>
-      <c r="E14" s="4" t="inlineStr"/>
-      <c r="F14" s="4" t="inlineStr"/>
-      <c r="G14" s="4" t="inlineStr"/>
-      <c r="H14" s="4" t="inlineStr"/>
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Bus_2</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr"/>
+      <c r="C14" s="3" t="inlineStr"/>
+      <c r="D14" s="3" t="inlineStr"/>
+      <c r="E14" s="3" t="inlineStr"/>
+      <c r="F14" s="3" t="inlineStr"/>
+      <c r="G14" s="3" t="inlineStr"/>
+      <c r="H14" s="3" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>Bus_2</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="inlineStr"/>
-      <c r="C15" s="3" t="inlineStr"/>
-      <c r="D15" s="3" t="inlineStr"/>
-      <c r="E15" s="3" t="inlineStr"/>
-      <c r="F15" s="3" t="inlineStr"/>
-      <c r="G15" s="3" t="inlineStr"/>
-      <c r="H15" s="3" t="inlineStr"/>
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Driver_1_12hr</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr"/>
+      <c r="C15" s="4" t="inlineStr"/>
+      <c r="D15" s="4" t="inlineStr"/>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>14:15 - 02:15</t>
+        </is>
+      </c>
+      <c r="F15" s="4" t="inlineStr"/>
+      <c r="G15" s="4" t="inlineStr"/>
+      <c r="H15" s="4" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Driver_5_8hr</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 14:15</t>
-        </is>
-      </c>
+          <t>Driver_4_8hr</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr"/>
       <c r="C16" s="4" t="inlineStr"/>
       <c r="D16" s="4" t="inlineStr"/>
-      <c r="E16" s="4" t="inlineStr"/>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 14:15</t>
+        </is>
+      </c>
       <c r="F16" s="4" t="inlineStr"/>
       <c r="G16" s="4" t="inlineStr"/>
       <c r="H16" s="4" t="inlineStr"/>
@@ -760,105 +764,109 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Driver_8_12hr</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
-        <is>
-          <t>14:15 - 02:15</t>
-        </is>
-      </c>
+          <t>Driver_5_8hr</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr"/>
       <c r="C17" s="4" t="inlineStr"/>
       <c r="D17" s="4" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr"/>
-      <c r="F17" s="4" t="inlineStr"/>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 14:15</t>
+        </is>
+      </c>
       <c r="G17" s="4" t="inlineStr"/>
       <c r="H17" s="4" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>Driver_13_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="inlineStr"/>
-      <c r="C18" s="4" t="inlineStr"/>
+          <t>Driver_9_12hr</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>14:15 - 02:15</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="inlineStr">
+        <is>
+          <t>14:15 - 02:15</t>
+        </is>
+      </c>
       <c r="D18" s="4" t="inlineStr"/>
       <c r="E18" s="4" t="inlineStr"/>
       <c r="F18" s="4" t="inlineStr"/>
-      <c r="G18" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 18:15</t>
-        </is>
-      </c>
+      <c r="G18" s="4" t="inlineStr"/>
       <c r="H18" s="4" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Driver_17_12hr</t>
+          <t>Driver_27_12hr_wk</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr"/>
       <c r="C19" s="4" t="inlineStr"/>
       <c r="D19" s="4" t="inlineStr"/>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>14:15 - 02:15</t>
-        </is>
-      </c>
+      <c r="E19" s="4" t="inlineStr"/>
       <c r="F19" s="4" t="inlineStr"/>
-      <c r="G19" s="4" t="inlineStr"/>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 18:15</t>
+        </is>
+      </c>
       <c r="H19" s="4" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Driver_31_12hr</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="inlineStr"/>
-      <c r="C20" s="4" t="inlineStr"/>
+          <t>Driver_32_8hr</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 14:15</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 14:15</t>
+        </is>
+      </c>
       <c r="D20" s="4" t="inlineStr"/>
       <c r="E20" s="4" t="inlineStr"/>
-      <c r="F20" s="4" t="inlineStr">
-        <is>
-          <t>14:15 - 02:15</t>
-        </is>
-      </c>
+      <c r="F20" s="4" t="inlineStr"/>
       <c r="G20" s="4" t="inlineStr"/>
       <c r="H20" s="4" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Driver_40_8hr</t>
+          <t>Driver_33_8hr</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr"/>
       <c r="C21" s="4" t="inlineStr"/>
-      <c r="D21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 14:15</t>
+        </is>
+      </c>
       <c r="E21" s="4" t="inlineStr"/>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 14:15</t>
-        </is>
-      </c>
+      <c r="F21" s="4" t="inlineStr"/>
       <c r="G21" s="4" t="inlineStr"/>
       <c r="H21" s="4" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Driver_45_12hr</t>
+          <t>Driver_37_12hr</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr"/>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>14:15 - 02:15</t>
-        </is>
-      </c>
+      <c r="C22" s="4" t="inlineStr"/>
       <c r="D22" s="4" t="inlineStr">
         <is>
           <t>14:15 - 02:15</t>
@@ -872,103 +880,103 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Driver_47_8hr</t>
+          <t>Driver_42_12hr_wk</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr"/>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 14:15</t>
-        </is>
-      </c>
+      <c r="C23" s="4" t="inlineStr"/>
       <c r="D23" s="4" t="inlineStr"/>
       <c r="E23" s="4" t="inlineStr"/>
       <c r="F23" s="4" t="inlineStr"/>
       <c r="G23" s="4" t="inlineStr"/>
-      <c r="H23" s="4" t="inlineStr"/>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
+          <t>06:15 - 18:15</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Driver_53_8hr</t>
+          <t>Driver_52_12hr</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr"/>
       <c r="C24" s="4" t="inlineStr"/>
       <c r="D24" s="4" t="inlineStr"/>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 14:15</t>
-        </is>
-      </c>
-      <c r="F24" s="4" t="inlineStr"/>
+      <c r="E24" s="4" t="inlineStr"/>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>14:15 - 02:15</t>
+        </is>
+      </c>
       <c r="G24" s="4" t="inlineStr"/>
       <c r="H24" s="4" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
-        <is>
-          <t>Driver_54_8hr</t>
-        </is>
-      </c>
-      <c r="B25" s="4" t="inlineStr"/>
-      <c r="C25" s="4" t="inlineStr"/>
-      <c r="D25" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 14:15</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="inlineStr"/>
-      <c r="F25" s="4" t="inlineStr"/>
-      <c r="G25" s="4" t="inlineStr"/>
-      <c r="H25" s="4" t="inlineStr"/>
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>Bus_3</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr"/>
+      <c r="C25" s="3" t="inlineStr"/>
+      <c r="D25" s="3" t="inlineStr"/>
+      <c r="E25" s="3" t="inlineStr"/>
+      <c r="F25" s="3" t="inlineStr"/>
+      <c r="G25" s="3" t="inlineStr"/>
+      <c r="H25" s="3" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Driver_56_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="inlineStr"/>
+          <t>Driver_2_12hr</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>14:30 - 02:30</t>
+        </is>
+      </c>
       <c r="C26" s="4" t="inlineStr"/>
       <c r="D26" s="4" t="inlineStr"/>
       <c r="E26" s="4" t="inlineStr"/>
       <c r="F26" s="4" t="inlineStr"/>
       <c r="G26" s="4" t="inlineStr"/>
-      <c r="H26" s="4" t="inlineStr">
-        <is>
-          <t>06:15 - 18:15</t>
-        </is>
-      </c>
+      <c r="H26" s="4" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="inlineStr">
-        <is>
-          <t>Bus_3</t>
-        </is>
-      </c>
-      <c r="B27" s="3" t="inlineStr"/>
-      <c r="C27" s="3" t="inlineStr"/>
-      <c r="D27" s="3" t="inlineStr"/>
-      <c r="E27" s="3" t="inlineStr"/>
-      <c r="F27" s="3" t="inlineStr"/>
-      <c r="G27" s="3" t="inlineStr"/>
-      <c r="H27" s="3" t="inlineStr"/>
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>Driver_13_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr"/>
+      <c r="C27" s="4" t="inlineStr"/>
+      <c r="D27" s="4" t="inlineStr"/>
+      <c r="E27" s="4" t="inlineStr"/>
+      <c r="F27" s="4" t="inlineStr"/>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>06:30 - 18:30</t>
+        </is>
+      </c>
+      <c r="H27" s="4" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Driver_3_12hr</t>
+          <t>Driver_15_12hr</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr"/>
       <c r="C28" s="4" t="inlineStr"/>
-      <c r="D28" s="4" t="inlineStr"/>
-      <c r="E28" s="4" t="inlineStr">
+      <c r="D28" s="4" t="inlineStr">
         <is>
           <t>14:30 - 02:30</t>
         </is>
       </c>
+      <c r="E28" s="4" t="inlineStr"/>
       <c r="F28" s="4" t="inlineStr"/>
       <c r="G28" s="4" t="inlineStr"/>
       <c r="H28" s="4" t="inlineStr"/>
@@ -976,69 +984,69 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Driver_14_12hr_wk</t>
+          <t>Driver_16_12hr</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr"/>
       <c r="C29" s="4" t="inlineStr"/>
       <c r="D29" s="4" t="inlineStr"/>
       <c r="E29" s="4" t="inlineStr"/>
-      <c r="F29" s="4" t="inlineStr"/>
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>14:30 - 02:30</t>
+        </is>
+      </c>
       <c r="G29" s="4" t="inlineStr"/>
-      <c r="H29" s="4" t="inlineStr">
-        <is>
-          <t>06:30 - 18:30</t>
-        </is>
-      </c>
+      <c r="H29" s="4" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Driver_16_12hr</t>
+          <t>Driver_17_12hr</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr"/>
-      <c r="C30" s="4" t="inlineStr"/>
+      <c r="C30" s="4" t="inlineStr">
+        <is>
+          <t>14:30 - 02:30</t>
+        </is>
+      </c>
       <c r="D30" s="4" t="inlineStr"/>
       <c r="E30" s="4" t="inlineStr"/>
-      <c r="F30" s="4" t="inlineStr">
-        <is>
-          <t>14:30 - 02:30</t>
-        </is>
-      </c>
+      <c r="F30" s="4" t="inlineStr"/>
       <c r="G30" s="4" t="inlineStr"/>
       <c r="H30" s="4" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Driver_27_12hr_wk</t>
+          <t>Driver_18_8hr</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr"/>
       <c r="C31" s="4" t="inlineStr"/>
       <c r="D31" s="4" t="inlineStr"/>
-      <c r="E31" s="4" t="inlineStr"/>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
+          <t>06:30 - 14:30</t>
+        </is>
+      </c>
       <c r="F31" s="4" t="inlineStr"/>
-      <c r="G31" s="4" t="inlineStr">
-        <is>
-          <t>06:30 - 18:30</t>
-        </is>
-      </c>
+      <c r="G31" s="4" t="inlineStr"/>
       <c r="H31" s="4" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Driver_30_12hr</t>
-        </is>
-      </c>
-      <c r="B32" s="4" t="inlineStr">
-        <is>
-          <t>14:30 - 02:30</t>
-        </is>
-      </c>
-      <c r="C32" s="4" t="inlineStr"/>
+          <t>Driver_19_8hr</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="inlineStr"/>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>06:30 - 14:30</t>
+        </is>
+      </c>
       <c r="D32" s="4" t="inlineStr"/>
       <c r="E32" s="4" t="inlineStr"/>
       <c r="F32" s="4" t="inlineStr"/>
@@ -1048,16 +1056,16 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Driver_32_8hr</t>
-        </is>
-      </c>
-      <c r="B33" s="4" t="inlineStr"/>
+          <t>Driver_40_8hr</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>06:30 - 14:30</t>
+        </is>
+      </c>
       <c r="C33" s="4" t="inlineStr"/>
-      <c r="D33" s="4" t="inlineStr">
-        <is>
-          <t>06:30 - 14:30</t>
-        </is>
-      </c>
+      <c r="D33" s="4" t="inlineStr"/>
       <c r="E33" s="4" t="inlineStr"/>
       <c r="F33" s="4" t="inlineStr"/>
       <c r="G33" s="4" t="inlineStr"/>
@@ -1066,21 +1074,17 @@
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Driver_33_8hr</t>
+          <t>Driver_46_8hr</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr"/>
-      <c r="C34" s="4" t="inlineStr">
+      <c r="C34" s="4" t="inlineStr"/>
+      <c r="D34" s="4" t="inlineStr">
         <is>
           <t>06:30 - 14:30</t>
         </is>
       </c>
-      <c r="D34" s="4" t="inlineStr"/>
-      <c r="E34" s="4" t="inlineStr">
-        <is>
-          <t>06:30 - 14:30</t>
-        </is>
-      </c>
+      <c r="E34" s="4" t="inlineStr"/>
       <c r="F34" s="4" t="inlineStr">
         <is>
           <t>06:30 - 14:30</t>
@@ -1092,84 +1096,84 @@
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Driver_37_12hr</t>
+          <t>Driver_49_12hr_wk</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr"/>
       <c r="C35" s="4" t="inlineStr"/>
-      <c r="D35" s="4" t="inlineStr">
-        <is>
-          <t>14:30 - 02:30</t>
-        </is>
-      </c>
+      <c r="D35" s="4" t="inlineStr"/>
       <c r="E35" s="4" t="inlineStr"/>
       <c r="F35" s="4" t="inlineStr"/>
       <c r="G35" s="4" t="inlineStr"/>
-      <c r="H35" s="4" t="inlineStr"/>
+      <c r="H35" s="4" t="inlineStr">
+        <is>
+          <t>06:30 - 18:30</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Driver_44_12hr</t>
+          <t>Driver_51_12hr</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr"/>
-      <c r="C36" s="4" t="inlineStr">
+      <c r="C36" s="4" t="inlineStr"/>
+      <c r="D36" s="4" t="inlineStr"/>
+      <c r="E36" s="4" t="inlineStr">
         <is>
           <t>14:30 - 02:30</t>
         </is>
       </c>
-      <c r="D36" s="4" t="inlineStr"/>
-      <c r="E36" s="4" t="inlineStr"/>
       <c r="F36" s="4" t="inlineStr"/>
       <c r="G36" s="4" t="inlineStr"/>
       <c r="H36" s="4" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
-        <is>
-          <t>Driver_53_8hr</t>
-        </is>
-      </c>
-      <c r="B37" s="4" t="inlineStr">
-        <is>
-          <t>06:30 - 14:30</t>
-        </is>
-      </c>
-      <c r="C37" s="4" t="inlineStr"/>
-      <c r="D37" s="4" t="inlineStr"/>
-      <c r="E37" s="4" t="inlineStr"/>
-      <c r="F37" s="4" t="inlineStr"/>
-      <c r="G37" s="4" t="inlineStr"/>
-      <c r="H37" s="4" t="inlineStr"/>
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>Bus_4</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr"/>
+      <c r="C37" s="3" t="inlineStr"/>
+      <c r="D37" s="3" t="inlineStr"/>
+      <c r="E37" s="3" t="inlineStr"/>
+      <c r="F37" s="3" t="inlineStr"/>
+      <c r="G37" s="3" t="inlineStr"/>
+      <c r="H37" s="3" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="inlineStr">
-        <is>
-          <t>Bus_4</t>
-        </is>
-      </c>
-      <c r="B38" s="3" t="inlineStr"/>
-      <c r="C38" s="3" t="inlineStr"/>
-      <c r="D38" s="3" t="inlineStr"/>
-      <c r="E38" s="3" t="inlineStr"/>
-      <c r="F38" s="3" t="inlineStr"/>
-      <c r="G38" s="3" t="inlineStr"/>
-      <c r="H38" s="3" t="inlineStr"/>
+      <c r="A38" s="4" t="inlineStr">
+        <is>
+          <t>Driver_1_12hr</t>
+        </is>
+      </c>
+      <c r="B38" s="4" t="inlineStr"/>
+      <c r="C38" s="4" t="inlineStr"/>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>14:45 - 02:45</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr"/>
+      <c r="F38" s="4" t="inlineStr"/>
+      <c r="G38" s="4" t="inlineStr"/>
+      <c r="H38" s="4" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Driver_4_8hr</t>
+          <t>Driver_5_8hr</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr"/>
-      <c r="C39" s="4" t="inlineStr"/>
-      <c r="D39" s="4" t="inlineStr">
+      <c r="C39" s="4" t="inlineStr">
         <is>
           <t>06:45 - 14:45</t>
         </is>
       </c>
+      <c r="D39" s="4" t="inlineStr"/>
       <c r="E39" s="4" t="inlineStr"/>
       <c r="F39" s="4" t="inlineStr"/>
       <c r="G39" s="4" t="inlineStr"/>
@@ -1178,61 +1182,61 @@
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Driver_9_12hr</t>
+          <t>Driver_6_12hr_wk</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr"/>
       <c r="C40" s="4" t="inlineStr"/>
-      <c r="D40" s="4" t="inlineStr">
-        <is>
-          <t>14:45 - 02:45</t>
-        </is>
-      </c>
+      <c r="D40" s="4" t="inlineStr"/>
       <c r="E40" s="4" t="inlineStr"/>
       <c r="F40" s="4" t="inlineStr"/>
-      <c r="G40" s="4" t="inlineStr"/>
+      <c r="G40" s="4" t="inlineStr">
+        <is>
+          <t>06:45 - 18:45</t>
+        </is>
+      </c>
       <c r="H40" s="4" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Driver_12_8hr</t>
+          <t>Driver_10_12hr</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr"/>
       <c r="C41" s="4" t="inlineStr"/>
       <c r="D41" s="4" t="inlineStr"/>
-      <c r="E41" s="4" t="inlineStr">
-        <is>
-          <t>06:45 - 14:45</t>
-        </is>
-      </c>
-      <c r="F41" s="4" t="inlineStr"/>
+      <c r="E41" s="4" t="inlineStr"/>
+      <c r="F41" s="4" t="inlineStr">
+        <is>
+          <t>14:45 - 02:45</t>
+        </is>
+      </c>
       <c r="G41" s="4" t="inlineStr"/>
       <c r="H41" s="4" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Driver_18_8hr</t>
-        </is>
-      </c>
-      <c r="B42" s="4" t="inlineStr">
-        <is>
-          <t>06:45 - 14:45</t>
-        </is>
-      </c>
+          <t>Driver_11_8hr</t>
+        </is>
+      </c>
+      <c r="B42" s="4" t="inlineStr"/>
       <c r="C42" s="4" t="inlineStr"/>
       <c r="D42" s="4" t="inlineStr"/>
       <c r="E42" s="4" t="inlineStr"/>
-      <c r="F42" s="4" t="inlineStr"/>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>06:45 - 14:45</t>
+        </is>
+      </c>
       <c r="G42" s="4" t="inlineStr"/>
       <c r="H42" s="4" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Driver_24_12hr</t>
+          <t>Driver_12_8hr</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr"/>
@@ -1240,7 +1244,7 @@
       <c r="D43" s="4" t="inlineStr"/>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t>14:45 - 02:45</t>
+          <t>06:45 - 14:45</t>
         </is>
       </c>
       <c r="F43" s="4" t="inlineStr"/>
@@ -1250,35 +1254,35 @@
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Driver_42_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="inlineStr"/>
+          <t>Driver_22_12hr</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>14:45 - 02:45</t>
+        </is>
+      </c>
       <c r="C44" s="4" t="inlineStr"/>
       <c r="D44" s="4" t="inlineStr"/>
       <c r="E44" s="4" t="inlineStr"/>
       <c r="F44" s="4" t="inlineStr"/>
       <c r="G44" s="4" t="inlineStr"/>
-      <c r="H44" s="4" t="inlineStr">
-        <is>
-          <t>06:45 - 18:45</t>
-        </is>
-      </c>
+      <c r="H44" s="4" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Driver_43_12hr</t>
-        </is>
-      </c>
-      <c r="B45" s="4" t="inlineStr">
-        <is>
-          <t>14:45 - 02:45</t>
-        </is>
-      </c>
+          <t>Driver_36_12hr</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="inlineStr"/>
       <c r="C45" s="4" t="inlineStr"/>
       <c r="D45" s="4" t="inlineStr"/>
-      <c r="E45" s="4" t="inlineStr"/>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>14:45 - 02:45</t>
+        </is>
+      </c>
       <c r="F45" s="4" t="inlineStr"/>
       <c r="G45" s="4" t="inlineStr"/>
       <c r="H45" s="4" t="inlineStr"/>
@@ -1286,34 +1290,34 @@
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Driver_44_12hr</t>
-        </is>
-      </c>
-      <c r="B46" s="4" t="inlineStr"/>
+          <t>Driver_39_8hr</t>
+        </is>
+      </c>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t>06:45 - 14:45</t>
+        </is>
+      </c>
       <c r="C46" s="4" t="inlineStr"/>
       <c r="D46" s="4" t="inlineStr"/>
       <c r="E46" s="4" t="inlineStr"/>
-      <c r="F46" s="4" t="inlineStr">
-        <is>
-          <t>14:45 - 02:45</t>
-        </is>
-      </c>
+      <c r="F46" s="4" t="inlineStr"/>
       <c r="G46" s="4" t="inlineStr"/>
       <c r="H46" s="4" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Driver_46_8hr</t>
+          <t>Driver_40_8hr</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr"/>
-      <c r="C47" s="4" t="inlineStr">
+      <c r="C47" s="4" t="inlineStr"/>
+      <c r="D47" s="4" t="inlineStr">
         <is>
           <t>06:45 - 14:45</t>
         </is>
       </c>
-      <c r="D47" s="4" t="inlineStr"/>
       <c r="E47" s="4" t="inlineStr"/>
       <c r="F47" s="4" t="inlineStr"/>
       <c r="G47" s="4" t="inlineStr"/>
@@ -1322,100 +1326,96 @@
     <row r="48">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Driver_47_8hr</t>
+          <t>Driver_43_12hr</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr"/>
-      <c r="C48" s="4" t="inlineStr"/>
+      <c r="C48" s="4" t="inlineStr">
+        <is>
+          <t>14:45 - 02:45</t>
+        </is>
+      </c>
       <c r="D48" s="4" t="inlineStr"/>
       <c r="E48" s="4" t="inlineStr"/>
-      <c r="F48" s="4" t="inlineStr">
-        <is>
-          <t>06:45 - 14:45</t>
-        </is>
-      </c>
+      <c r="F48" s="4" t="inlineStr"/>
       <c r="G48" s="4" t="inlineStr"/>
       <c r="H48" s="4" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Driver_50_12hr</t>
+          <t>Driver_56_12hr_wk</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr"/>
-      <c r="C49" s="4" t="inlineStr">
-        <is>
-          <t>14:45 - 02:45</t>
-        </is>
-      </c>
+      <c r="C49" s="4" t="inlineStr"/>
       <c r="D49" s="4" t="inlineStr"/>
       <c r="E49" s="4" t="inlineStr"/>
       <c r="F49" s="4" t="inlineStr"/>
       <c r="G49" s="4" t="inlineStr"/>
-      <c r="H49" s="4" t="inlineStr"/>
+      <c r="H49" s="4" t="inlineStr">
+        <is>
+          <t>06:45 - 18:45</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="inlineStr">
-        <is>
-          <t>Driver_55_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B50" s="4" t="inlineStr"/>
-      <c r="C50" s="4" t="inlineStr"/>
-      <c r="D50" s="4" t="inlineStr"/>
-      <c r="E50" s="4" t="inlineStr"/>
-      <c r="F50" s="4" t="inlineStr"/>
-      <c r="G50" s="4" t="inlineStr">
-        <is>
-          <t>06:45 - 18:45</t>
-        </is>
-      </c>
-      <c r="H50" s="4" t="inlineStr"/>
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>Bus_5</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="inlineStr"/>
+      <c r="C50" s="3" t="inlineStr"/>
+      <c r="D50" s="3" t="inlineStr"/>
+      <c r="E50" s="3" t="inlineStr"/>
+      <c r="F50" s="3" t="inlineStr"/>
+      <c r="G50" s="3" t="inlineStr"/>
+      <c r="H50" s="3" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="inlineStr">
-        <is>
-          <t>Bus_5</t>
-        </is>
-      </c>
-      <c r="B51" s="3" t="inlineStr"/>
-      <c r="C51" s="3" t="inlineStr"/>
-      <c r="D51" s="3" t="inlineStr"/>
-      <c r="E51" s="3" t="inlineStr"/>
-      <c r="F51" s="3" t="inlineStr"/>
-      <c r="G51" s="3" t="inlineStr"/>
-      <c r="H51" s="3" t="inlineStr"/>
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>Driver_3_12hr</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr"/>
+      <c r="C51" s="4" t="inlineStr"/>
+      <c r="D51" s="4" t="inlineStr"/>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>17:00 - 05:00</t>
+        </is>
+      </c>
+      <c r="F51" s="4" t="inlineStr"/>
+      <c r="G51" s="4" t="inlineStr"/>
+      <c r="H51" s="4" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Driver_1_12hr</t>
+          <t>Driver_8_12hr</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr"/>
       <c r="C52" s="4" t="inlineStr"/>
       <c r="D52" s="4" t="inlineStr"/>
-      <c r="E52" s="4" t="inlineStr">
+      <c r="E52" s="4" t="inlineStr"/>
+      <c r="F52" s="4" t="inlineStr">
         <is>
           <t>17:00 - 05:00</t>
         </is>
       </c>
-      <c r="F52" s="4" t="inlineStr"/>
       <c r="G52" s="4" t="inlineStr"/>
       <c r="H52" s="4" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Driver_4_8hr</t>
-        </is>
-      </c>
-      <c r="B53" s="4" t="inlineStr">
-        <is>
-          <t>09:00 - 17:00</t>
-        </is>
-      </c>
+          <t>Driver_11_8hr</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="inlineStr"/>
       <c r="C53" s="4" t="inlineStr"/>
       <c r="D53" s="4" t="inlineStr"/>
       <c r="E53" s="4" t="inlineStr">
@@ -1430,52 +1430,52 @@
     <row r="54">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>Driver_7_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B54" s="4" t="inlineStr"/>
+          <t>Driver_25_8hr</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>09:00 - 17:00</t>
+        </is>
+      </c>
       <c r="C54" s="4" t="inlineStr"/>
       <c r="D54" s="4" t="inlineStr"/>
       <c r="E54" s="4" t="inlineStr"/>
       <c r="F54" s="4" t="inlineStr"/>
       <c r="G54" s="4" t="inlineStr"/>
-      <c r="H54" s="4" t="inlineStr">
-        <is>
-          <t>18:03 - 06:03</t>
-        </is>
-      </c>
+      <c r="H54" s="4" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Driver_11_8hr</t>
+          <t>Driver_28_12hr_wk</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr"/>
-      <c r="C55" s="4" t="inlineStr">
-        <is>
-          <t>09:00 - 17:00</t>
-        </is>
-      </c>
+      <c r="C55" s="4" t="inlineStr"/>
       <c r="D55" s="4" t="inlineStr"/>
       <c r="E55" s="4" t="inlineStr"/>
       <c r="F55" s="4" t="inlineStr"/>
       <c r="G55" s="4" t="inlineStr"/>
-      <c r="H55" s="4" t="inlineStr"/>
+      <c r="H55" s="4" t="inlineStr">
+        <is>
+          <t>18:03 - 06:03</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>Driver_16_12hr</t>
-        </is>
-      </c>
-      <c r="B56" s="4" t="inlineStr">
+          <t>Driver_30_12hr</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr"/>
+      <c r="C56" s="4" t="inlineStr"/>
+      <c r="D56" s="4" t="inlineStr">
         <is>
           <t>17:00 - 05:00</t>
         </is>
       </c>
-      <c r="C56" s="4" t="inlineStr"/>
-      <c r="D56" s="4" t="inlineStr"/>
       <c r="E56" s="4" t="inlineStr"/>
       <c r="F56" s="4" t="inlineStr"/>
       <c r="G56" s="4" t="inlineStr"/>
@@ -1484,129 +1484,133 @@
     <row r="57">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>Driver_19_8hr</t>
+          <t>Driver_34_12hr_wk</t>
         </is>
       </c>
       <c r="B57" s="4" t="inlineStr"/>
       <c r="C57" s="4" t="inlineStr"/>
-      <c r="D57" s="4" t="inlineStr">
-        <is>
-          <t>09:00 - 17:00</t>
-        </is>
-      </c>
+      <c r="D57" s="4" t="inlineStr"/>
       <c r="E57" s="4" t="inlineStr"/>
       <c r="F57" s="4" t="inlineStr"/>
-      <c r="G57" s="4" t="inlineStr"/>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>18:03 - 06:03</t>
+        </is>
+      </c>
       <c r="H57" s="4" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>Driver_20_12hr_wk</t>
+          <t>Driver_39_8hr</t>
         </is>
       </c>
       <c r="B58" s="4" t="inlineStr"/>
       <c r="C58" s="4" t="inlineStr"/>
-      <c r="D58" s="4" t="inlineStr"/>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>09:00 - 17:00</t>
+        </is>
+      </c>
       <c r="E58" s="4" t="inlineStr"/>
       <c r="F58" s="4" t="inlineStr"/>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>18:03 - 06:03</t>
-        </is>
-      </c>
+      <c r="G58" s="4" t="inlineStr"/>
       <c r="H58" s="4" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>Driver_24_12hr</t>
+          <t>Driver_40_8hr</t>
         </is>
       </c>
       <c r="B59" s="4" t="inlineStr"/>
-      <c r="C59" s="4" t="inlineStr">
-        <is>
-          <t>17:00 - 05:00</t>
-        </is>
-      </c>
+      <c r="C59" s="4" t="inlineStr"/>
       <c r="D59" s="4" t="inlineStr"/>
       <c r="E59" s="4" t="inlineStr"/>
-      <c r="F59" s="4" t="inlineStr"/>
+      <c r="F59" s="4" t="inlineStr">
+        <is>
+          <t>09:00 - 17:00</t>
+        </is>
+      </c>
       <c r="G59" s="4" t="inlineStr"/>
       <c r="H59" s="4" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="4" t="inlineStr">
         <is>
-          <t>Driver_26_8hr</t>
-        </is>
-      </c>
-      <c r="B60" s="4" t="inlineStr"/>
-      <c r="C60" s="4" t="inlineStr"/>
+          <t>Driver_44_12hr</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>17:00 - 05:00</t>
+        </is>
+      </c>
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>17:00 - 05:00</t>
+        </is>
+      </c>
       <c r="D60" s="4" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr"/>
-      <c r="F60" s="4" t="inlineStr">
-        <is>
-          <t>09:00 - 17:00</t>
-        </is>
-      </c>
+      <c r="F60" s="4" t="inlineStr"/>
       <c r="G60" s="4" t="inlineStr"/>
       <c r="H60" s="4" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>Driver_36_12hr</t>
+          <t>Driver_46_8hr</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr"/>
-      <c r="C61" s="4" t="inlineStr"/>
-      <c r="D61" s="4" t="inlineStr">
-        <is>
-          <t>17:00 - 05:00</t>
-        </is>
-      </c>
+      <c r="C61" s="4" t="inlineStr">
+        <is>
+          <t>09:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="D61" s="4" t="inlineStr"/>
       <c r="E61" s="4" t="inlineStr"/>
       <c r="F61" s="4" t="inlineStr"/>
       <c r="G61" s="4" t="inlineStr"/>
       <c r="H61" s="4" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="inlineStr">
-        <is>
-          <t>Driver_38_12hr</t>
-        </is>
-      </c>
-      <c r="B62" s="4" t="inlineStr"/>
-      <c r="C62" s="4" t="inlineStr"/>
-      <c r="D62" s="4" t="inlineStr"/>
-      <c r="E62" s="4" t="inlineStr"/>
-      <c r="F62" s="4" t="inlineStr">
-        <is>
-          <t>17:00 - 05:00</t>
-        </is>
-      </c>
-      <c r="G62" s="4" t="inlineStr"/>
-      <c r="H62" s="4" t="inlineStr"/>
+      <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>Bus_6</t>
+        </is>
+      </c>
+      <c r="B62" s="3" t="inlineStr"/>
+      <c r="C62" s="3" t="inlineStr"/>
+      <c r="D62" s="3" t="inlineStr"/>
+      <c r="E62" s="3" t="inlineStr"/>
+      <c r="F62" s="3" t="inlineStr"/>
+      <c r="G62" s="3" t="inlineStr"/>
+      <c r="H62" s="3" t="inlineStr"/>
     </row>
     <row r="63">
-      <c r="A63" s="3" t="inlineStr">
-        <is>
-          <t>Bus_6</t>
-        </is>
-      </c>
-      <c r="B63" s="3" t="inlineStr"/>
-      <c r="C63" s="3" t="inlineStr"/>
-      <c r="D63" s="3" t="inlineStr"/>
-      <c r="E63" s="3" t="inlineStr"/>
-      <c r="F63" s="3" t="inlineStr"/>
-      <c r="G63" s="3" t="inlineStr"/>
-      <c r="H63" s="3" t="inlineStr"/>
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>Driver_12_8hr</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="inlineStr"/>
+      <c r="C63" s="4" t="inlineStr"/>
+      <c r="D63" s="4" t="inlineStr">
+        <is>
+          <t>09:15 - 17:15</t>
+        </is>
+      </c>
+      <c r="E63" s="4" t="inlineStr"/>
+      <c r="F63" s="4" t="inlineStr"/>
+      <c r="G63" s="4" t="inlineStr"/>
+      <c r="H63" s="4" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="4" t="inlineStr">
         <is>
-          <t>Driver_6_12hr_wk</t>
+          <t>Driver_14_12hr_wk</t>
         </is>
       </c>
       <c r="B64" s="4" t="inlineStr"/>
@@ -1614,44 +1618,44 @@
       <c r="D64" s="4" t="inlineStr"/>
       <c r="E64" s="4" t="inlineStr"/>
       <c r="F64" s="4" t="inlineStr"/>
-      <c r="G64" s="4" t="inlineStr">
+      <c r="G64" s="4" t="inlineStr"/>
+      <c r="H64" s="4" t="inlineStr">
         <is>
           <t>18:18 - 06:18</t>
         </is>
       </c>
-      <c r="H64" s="4" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="4" t="inlineStr">
         <is>
-          <t>Driver_11_8hr</t>
+          <t>Driver_25_8hr</t>
         </is>
       </c>
       <c r="B65" s="4" t="inlineStr"/>
-      <c r="C65" s="4" t="inlineStr"/>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>09:15 - 17:15</t>
+        </is>
+      </c>
       <c r="D65" s="4" t="inlineStr"/>
       <c r="E65" s="4" t="inlineStr"/>
-      <c r="F65" s="4" t="inlineStr">
-        <is>
-          <t>09:15 - 17:15</t>
-        </is>
-      </c>
+      <c r="F65" s="4" t="inlineStr"/>
       <c r="G65" s="4" t="inlineStr"/>
       <c r="H65" s="4" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="4" t="inlineStr">
         <is>
-          <t>Driver_12_8hr</t>
-        </is>
-      </c>
-      <c r="B66" s="4" t="inlineStr"/>
+          <t>Driver_26_8hr</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>09:15 - 17:15</t>
+        </is>
+      </c>
       <c r="C66" s="4" t="inlineStr"/>
-      <c r="D66" s="4" t="inlineStr">
-        <is>
-          <t>09:15 - 17:15</t>
-        </is>
-      </c>
+      <c r="D66" s="4" t="inlineStr"/>
       <c r="E66" s="4" t="inlineStr"/>
       <c r="F66" s="4" t="inlineStr"/>
       <c r="G66" s="4" t="inlineStr"/>
@@ -1660,89 +1664,89 @@
     <row r="67">
       <c r="A67" s="4" t="inlineStr">
         <is>
-          <t>Driver_31_12hr</t>
+          <t>Driver_36_12hr</t>
         </is>
       </c>
       <c r="B67" s="4" t="inlineStr"/>
       <c r="C67" s="4" t="inlineStr"/>
       <c r="D67" s="4" t="inlineStr"/>
-      <c r="E67" s="4" t="inlineStr">
+      <c r="E67" s="4" t="inlineStr"/>
+      <c r="F67" s="4" t="inlineStr">
         <is>
           <t>17:15 - 05:15</t>
         </is>
       </c>
-      <c r="F67" s="4" t="inlineStr"/>
       <c r="G67" s="4" t="inlineStr"/>
       <c r="H67" s="4" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="4" t="inlineStr">
         <is>
-          <t>Driver_35_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B68" s="4" t="inlineStr"/>
+          <t>Driver_37_12hr</t>
+        </is>
+      </c>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>17:15 - 05:15</t>
+        </is>
+      </c>
       <c r="C68" s="4" t="inlineStr"/>
       <c r="D68" s="4" t="inlineStr"/>
       <c r="E68" s="4" t="inlineStr"/>
       <c r="F68" s="4" t="inlineStr"/>
       <c r="G68" s="4" t="inlineStr"/>
-      <c r="H68" s="4" t="inlineStr">
-        <is>
-          <t>18:18 - 06:18</t>
-        </is>
-      </c>
+      <c r="H68" s="4" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>Driver_36_12hr</t>
+          <t>Driver_39_8hr</t>
         </is>
       </c>
       <c r="B69" s="4" t="inlineStr"/>
-      <c r="C69" s="4" t="inlineStr">
-        <is>
-          <t>17:15 - 05:15</t>
-        </is>
-      </c>
+      <c r="C69" s="4" t="inlineStr"/>
       <c r="D69" s="4" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr"/>
-      <c r="F69" s="4" t="inlineStr"/>
+      <c r="F69" s="4" t="inlineStr">
+        <is>
+          <t>09:15 - 17:15</t>
+        </is>
+      </c>
       <c r="G69" s="4" t="inlineStr"/>
       <c r="H69" s="4" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="4" t="inlineStr">
         <is>
-          <t>Driver_37_12hr</t>
-        </is>
-      </c>
-      <c r="B70" s="4" t="inlineStr">
-        <is>
-          <t>17:15 - 05:15</t>
-        </is>
-      </c>
+          <t>Driver_41_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B70" s="4" t="inlineStr"/>
       <c r="C70" s="4" t="inlineStr"/>
       <c r="D70" s="4" t="inlineStr"/>
       <c r="E70" s="4" t="inlineStr"/>
       <c r="F70" s="4" t="inlineStr"/>
-      <c r="G70" s="4" t="inlineStr"/>
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>18:18 - 06:18</t>
+        </is>
+      </c>
       <c r="H70" s="4" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="4" t="inlineStr">
         <is>
-          <t>Driver_38_12hr</t>
+          <t>Driver_47_8hr</t>
         </is>
       </c>
       <c r="B71" s="4" t="inlineStr"/>
       <c r="C71" s="4" t="inlineStr"/>
-      <c r="D71" s="4" t="inlineStr">
-        <is>
-          <t>17:15 - 05:15</t>
-        </is>
-      </c>
-      <c r="E71" s="4" t="inlineStr"/>
+      <c r="D71" s="4" t="inlineStr"/>
+      <c r="E71" s="4" t="inlineStr">
+        <is>
+          <t>09:15 - 17:15</t>
+        </is>
+      </c>
       <c r="F71" s="4" t="inlineStr"/>
       <c r="G71" s="4" t="inlineStr"/>
       <c r="H71" s="4" t="inlineStr"/>
@@ -1750,17 +1754,17 @@
     <row r="72">
       <c r="A72" s="4" t="inlineStr">
         <is>
-          <t>Driver_47_8hr</t>
+          <t>Driver_50_12hr</t>
         </is>
       </c>
       <c r="B72" s="4" t="inlineStr"/>
-      <c r="C72" s="4" t="inlineStr"/>
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>17:15 - 05:15</t>
+        </is>
+      </c>
       <c r="D72" s="4" t="inlineStr"/>
-      <c r="E72" s="4" t="inlineStr">
-        <is>
-          <t>09:15 - 17:15</t>
-        </is>
-      </c>
+      <c r="E72" s="4" t="inlineStr"/>
       <c r="F72" s="4" t="inlineStr"/>
       <c r="G72" s="4" t="inlineStr"/>
       <c r="H72" s="4" t="inlineStr"/>
@@ -1773,82 +1777,78 @@
       </c>
       <c r="B73" s="4" t="inlineStr"/>
       <c r="C73" s="4" t="inlineStr"/>
-      <c r="D73" s="4" t="inlineStr"/>
+      <c r="D73" s="4" t="inlineStr">
+        <is>
+          <t>17:15 - 05:15</t>
+        </is>
+      </c>
       <c r="E73" s="4" t="inlineStr"/>
-      <c r="F73" s="4" t="inlineStr">
-        <is>
-          <t>17:15 - 05:15</t>
-        </is>
-      </c>
+      <c r="F73" s="4" t="inlineStr"/>
       <c r="G73" s="4" t="inlineStr"/>
       <c r="H73" s="4" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="4" t="inlineStr">
         <is>
-          <t>Driver_53_8hr</t>
+          <t>Driver_52_12hr</t>
         </is>
       </c>
       <c r="B74" s="4" t="inlineStr"/>
-      <c r="C74" s="4" t="inlineStr">
-        <is>
-          <t>09:15 - 17:15</t>
-        </is>
-      </c>
+      <c r="C74" s="4" t="inlineStr"/>
       <c r="D74" s="4" t="inlineStr"/>
-      <c r="E74" s="4" t="inlineStr"/>
+      <c r="E74" s="4" t="inlineStr">
+        <is>
+          <t>17:15 - 05:15</t>
+        </is>
+      </c>
       <c r="F74" s="4" t="inlineStr"/>
       <c r="G74" s="4" t="inlineStr"/>
       <c r="H74" s="4" t="inlineStr"/>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="inlineStr">
-        <is>
-          <t>Driver_54_8hr</t>
-        </is>
-      </c>
-      <c r="B75" s="4" t="inlineStr">
-        <is>
-          <t>09:15 - 17:15</t>
-        </is>
-      </c>
-      <c r="C75" s="4" t="inlineStr"/>
-      <c r="D75" s="4" t="inlineStr"/>
-      <c r="E75" s="4" t="inlineStr"/>
-      <c r="F75" s="4" t="inlineStr"/>
-      <c r="G75" s="4" t="inlineStr"/>
-      <c r="H75" s="4" t="inlineStr"/>
+      <c r="A75" s="3" t="inlineStr">
+        <is>
+          <t>Bus_7</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="inlineStr"/>
+      <c r="C75" s="3" t="inlineStr"/>
+      <c r="D75" s="3" t="inlineStr"/>
+      <c r="E75" s="3" t="inlineStr"/>
+      <c r="F75" s="3" t="inlineStr"/>
+      <c r="G75" s="3" t="inlineStr"/>
+      <c r="H75" s="3" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" s="3" t="inlineStr">
-        <is>
-          <t>Bus_7</t>
-        </is>
-      </c>
-      <c r="B76" s="3" t="inlineStr"/>
-      <c r="C76" s="3" t="inlineStr"/>
-      <c r="D76" s="3" t="inlineStr"/>
-      <c r="E76" s="3" t="inlineStr"/>
-      <c r="F76" s="3" t="inlineStr"/>
-      <c r="G76" s="3" t="inlineStr"/>
-      <c r="H76" s="3" t="inlineStr"/>
+      <c r="A76" s="4" t="inlineStr">
+        <is>
+          <t>Driver_4_8hr</t>
+        </is>
+      </c>
+      <c r="B76" s="4" t="inlineStr"/>
+      <c r="C76" s="4" t="inlineStr">
+        <is>
+          <t>09:30 - 17:30</t>
+        </is>
+      </c>
+      <c r="D76" s="4" t="inlineStr"/>
+      <c r="E76" s="4" t="inlineStr"/>
+      <c r="F76" s="4" t="inlineStr"/>
+      <c r="G76" s="4" t="inlineStr"/>
+      <c r="H76" s="4" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>Driver_11_8hr</t>
+          <t>Driver_8_12hr</t>
         </is>
       </c>
       <c r="B77" s="4" t="inlineStr"/>
       <c r="C77" s="4" t="inlineStr"/>
-      <c r="D77" s="4" t="inlineStr">
-        <is>
-          <t>09:30 - 17:30</t>
-        </is>
-      </c>
+      <c r="D77" s="4" t="inlineStr"/>
       <c r="E77" s="4" t="inlineStr">
         <is>
-          <t>09:30 - 17:30</t>
+          <t>17:30 - 05:30</t>
         </is>
       </c>
       <c r="F77" s="4" t="inlineStr"/>
@@ -1858,17 +1858,17 @@
     <row r="78">
       <c r="A78" s="4" t="inlineStr">
         <is>
-          <t>Driver_16_12hr</t>
-        </is>
-      </c>
-      <c r="B78" s="4" t="inlineStr"/>
+          <t>Driver_11_8hr</t>
+        </is>
+      </c>
+      <c r="B78" s="4" t="inlineStr">
+        <is>
+          <t>09:30 - 17:30</t>
+        </is>
+      </c>
       <c r="C78" s="4" t="inlineStr"/>
       <c r="D78" s="4" t="inlineStr"/>
-      <c r="E78" s="4" t="inlineStr">
-        <is>
-          <t>17:30 - 05:30</t>
-        </is>
-      </c>
+      <c r="E78" s="4" t="inlineStr"/>
       <c r="F78" s="4" t="inlineStr"/>
       <c r="G78" s="4" t="inlineStr"/>
       <c r="H78" s="4" t="inlineStr"/>
@@ -1876,38 +1876,34 @@
     <row r="79">
       <c r="A79" s="4" t="inlineStr">
         <is>
-          <t>Driver_18_8hr</t>
+          <t>Driver_21_12hr_wk</t>
         </is>
       </c>
       <c r="B79" s="4" t="inlineStr"/>
-      <c r="C79" s="4" t="inlineStr">
-        <is>
-          <t>09:30 - 17:30</t>
-        </is>
-      </c>
+      <c r="C79" s="4" t="inlineStr"/>
       <c r="D79" s="4" t="inlineStr"/>
       <c r="E79" s="4" t="inlineStr"/>
       <c r="F79" s="4" t="inlineStr"/>
       <c r="G79" s="4" t="inlineStr"/>
-      <c r="H79" s="4" t="inlineStr"/>
+      <c r="H79" s="4" t="inlineStr">
+        <is>
+          <t>18:33 - 06:33</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="4" t="inlineStr">
         <is>
-          <t>Driver_24_12hr</t>
-        </is>
-      </c>
-      <c r="B80" s="4" t="inlineStr">
+          <t>Driver_29_12hr</t>
+        </is>
+      </c>
+      <c r="B80" s="4" t="inlineStr"/>
+      <c r="C80" s="4" t="inlineStr">
         <is>
           <t>17:30 - 05:30</t>
         </is>
       </c>
-      <c r="C80" s="4" t="inlineStr"/>
-      <c r="D80" s="4" t="inlineStr">
-        <is>
-          <t>17:30 - 05:30</t>
-        </is>
-      </c>
+      <c r="D80" s="4" t="inlineStr"/>
       <c r="E80" s="4" t="inlineStr"/>
       <c r="F80" s="4" t="inlineStr"/>
       <c r="G80" s="4" t="inlineStr"/>
@@ -1916,88 +1912,88 @@
     <row r="81">
       <c r="A81" s="4" t="inlineStr">
         <is>
-          <t>Driver_28_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B81" s="4" t="inlineStr"/>
+          <t>Driver_31_12hr</t>
+        </is>
+      </c>
+      <c r="B81" s="4" t="inlineStr">
+        <is>
+          <t>17:30 - 05:30</t>
+        </is>
+      </c>
       <c r="C81" s="4" t="inlineStr"/>
       <c r="D81" s="4" t="inlineStr"/>
       <c r="E81" s="4" t="inlineStr"/>
       <c r="F81" s="4" t="inlineStr"/>
       <c r="G81" s="4" t="inlineStr"/>
-      <c r="H81" s="4" t="inlineStr">
-        <is>
-          <t>18:33 - 06:33</t>
-        </is>
-      </c>
+      <c r="H81" s="4" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="4" t="inlineStr">
         <is>
-          <t>Driver_33_8hr</t>
-        </is>
-      </c>
-      <c r="B82" s="4" t="inlineStr">
-        <is>
-          <t>09:30 - 17:30</t>
-        </is>
-      </c>
+          <t>Driver_38_12hr</t>
+        </is>
+      </c>
+      <c r="B82" s="4" t="inlineStr"/>
       <c r="C82" s="4" t="inlineStr"/>
       <c r="D82" s="4" t="inlineStr"/>
       <c r="E82" s="4" t="inlineStr"/>
-      <c r="F82" s="4" t="inlineStr"/>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>17:30 - 05:30</t>
+        </is>
+      </c>
       <c r="G82" s="4" t="inlineStr"/>
       <c r="H82" s="4" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="4" t="inlineStr">
         <is>
-          <t>Driver_36_12hr</t>
+          <t>Driver_40_8hr</t>
         </is>
       </c>
       <c r="B83" s="4" t="inlineStr"/>
       <c r="C83" s="4" t="inlineStr"/>
       <c r="D83" s="4" t="inlineStr"/>
-      <c r="E83" s="4" t="inlineStr"/>
-      <c r="F83" s="4" t="inlineStr">
-        <is>
-          <t>17:30 - 05:30</t>
-        </is>
-      </c>
+      <c r="E83" s="4" t="inlineStr">
+        <is>
+          <t>09:30 - 17:30</t>
+        </is>
+      </c>
+      <c r="F83" s="4" t="inlineStr"/>
       <c r="G83" s="4" t="inlineStr"/>
       <c r="H83" s="4" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="4" t="inlineStr">
         <is>
-          <t>Driver_48_12hr_wk</t>
+          <t>Driver_43_12hr</t>
         </is>
       </c>
       <c r="B84" s="4" t="inlineStr"/>
       <c r="C84" s="4" t="inlineStr"/>
-      <c r="D84" s="4" t="inlineStr"/>
+      <c r="D84" s="4" t="inlineStr">
+        <is>
+          <t>17:30 - 05:30</t>
+        </is>
+      </c>
       <c r="E84" s="4" t="inlineStr"/>
       <c r="F84" s="4" t="inlineStr"/>
-      <c r="G84" s="4" t="inlineStr">
-        <is>
-          <t>18:33 - 06:33</t>
-        </is>
-      </c>
+      <c r="G84" s="4" t="inlineStr"/>
       <c r="H84" s="4" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="4" t="inlineStr">
         <is>
-          <t>Driver_51_12hr</t>
+          <t>Driver_47_8hr</t>
         </is>
       </c>
       <c r="B85" s="4" t="inlineStr"/>
-      <c r="C85" s="4" t="inlineStr">
-        <is>
-          <t>17:30 - 05:30</t>
-        </is>
-      </c>
-      <c r="D85" s="4" t="inlineStr"/>
+      <c r="C85" s="4" t="inlineStr"/>
+      <c r="D85" s="4" t="inlineStr">
+        <is>
+          <t>09:30 - 17:30</t>
+        </is>
+      </c>
       <c r="E85" s="4" t="inlineStr"/>
       <c r="F85" s="4" t="inlineStr"/>
       <c r="G85" s="4" t="inlineStr"/>
@@ -2006,7 +2002,7 @@
     <row r="86">
       <c r="A86" s="4" t="inlineStr">
         <is>
-          <t>Driver_53_8hr</t>
+          <t>Driver_54_8hr</t>
         </is>
       </c>
       <c r="B86" s="4" t="inlineStr"/>
@@ -2022,41 +2018,41 @@
       <c r="H86" s="4" t="inlineStr"/>
     </row>
     <row r="87">
-      <c r="A87" s="3" t="inlineStr">
+      <c r="A87" s="4" t="inlineStr">
+        <is>
+          <t>Driver_55_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B87" s="4" t="inlineStr"/>
+      <c r="C87" s="4" t="inlineStr"/>
+      <c r="D87" s="4" t="inlineStr"/>
+      <c r="E87" s="4" t="inlineStr"/>
+      <c r="F87" s="4" t="inlineStr"/>
+      <c r="G87" s="4" t="inlineStr">
+        <is>
+          <t>18:33 - 06:33</t>
+        </is>
+      </c>
+      <c r="H87" s="4" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="inlineStr">
         <is>
           <t>Bus_8</t>
         </is>
       </c>
-      <c r="B87" s="3" t="inlineStr"/>
-      <c r="C87" s="3" t="inlineStr"/>
-      <c r="D87" s="3" t="inlineStr"/>
-      <c r="E87" s="3" t="inlineStr"/>
-      <c r="F87" s="3" t="inlineStr"/>
-      <c r="G87" s="3" t="inlineStr"/>
-      <c r="H87" s="3" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="4" t="inlineStr">
-        <is>
-          <t>Driver_23_12hr</t>
-        </is>
-      </c>
-      <c r="B88" s="4" t="inlineStr">
-        <is>
-          <t>17:45 - 05:45</t>
-        </is>
-      </c>
-      <c r="C88" s="4" t="inlineStr"/>
-      <c r="D88" s="4" t="inlineStr"/>
-      <c r="E88" s="4" t="inlineStr"/>
-      <c r="F88" s="4" t="inlineStr"/>
-      <c r="G88" s="4" t="inlineStr"/>
-      <c r="H88" s="4" t="inlineStr"/>
+      <c r="B88" s="3" t="inlineStr"/>
+      <c r="C88" s="3" t="inlineStr"/>
+      <c r="D88" s="3" t="inlineStr"/>
+      <c r="E88" s="3" t="inlineStr"/>
+      <c r="F88" s="3" t="inlineStr"/>
+      <c r="G88" s="3" t="inlineStr"/>
+      <c r="H88" s="3" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="4" t="inlineStr">
         <is>
-          <t>Driver_25_8hr</t>
+          <t>Driver_2_12hr</t>
         </is>
       </c>
       <c r="B89" s="4" t="inlineStr"/>
@@ -2065,7 +2061,7 @@
       <c r="E89" s="4" t="inlineStr"/>
       <c r="F89" s="4" t="inlineStr">
         <is>
-          <t>09:45 - 17:45</t>
+          <t>17:45 - 05:45</t>
         </is>
       </c>
       <c r="G89" s="4" t="inlineStr"/>
@@ -2074,17 +2070,17 @@
     <row r="90">
       <c r="A90" s="4" t="inlineStr">
         <is>
-          <t>Driver_26_8hr</t>
-        </is>
-      </c>
-      <c r="B90" s="4" t="inlineStr"/>
+          <t>Driver_5_8hr</t>
+        </is>
+      </c>
+      <c r="B90" s="4" t="inlineStr">
+        <is>
+          <t>09:45 - 17:45</t>
+        </is>
+      </c>
       <c r="C90" s="4" t="inlineStr"/>
       <c r="D90" s="4" t="inlineStr"/>
-      <c r="E90" s="4" t="inlineStr">
-        <is>
-          <t>09:45 - 17:45</t>
-        </is>
-      </c>
+      <c r="E90" s="4" t="inlineStr"/>
       <c r="F90" s="4" t="inlineStr"/>
       <c r="G90" s="4" t="inlineStr"/>
       <c r="H90" s="4" t="inlineStr"/>
@@ -2092,35 +2088,35 @@
     <row r="91">
       <c r="A91" s="4" t="inlineStr">
         <is>
-          <t>Driver_29_12hr</t>
+          <t>Driver_20_12hr_wk</t>
         </is>
       </c>
       <c r="B91" s="4" t="inlineStr"/>
-      <c r="C91" s="4" t="inlineStr">
-        <is>
-          <t>17:45 - 05:45</t>
-        </is>
-      </c>
+      <c r="C91" s="4" t="inlineStr"/>
       <c r="D91" s="4" t="inlineStr"/>
       <c r="E91" s="4" t="inlineStr"/>
       <c r="F91" s="4" t="inlineStr"/>
-      <c r="G91" s="4" t="inlineStr"/>
+      <c r="G91" s="4" t="inlineStr">
+        <is>
+          <t>18:48 - 06:48</t>
+        </is>
+      </c>
       <c r="H91" s="4" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="4" t="inlineStr">
         <is>
-          <t>Driver_33_8hr</t>
+          <t>Driver_22_12hr</t>
         </is>
       </c>
       <c r="B92" s="4" t="inlineStr"/>
       <c r="C92" s="4" t="inlineStr"/>
-      <c r="D92" s="4" t="inlineStr">
-        <is>
-          <t>09:45 - 17:45</t>
-        </is>
-      </c>
-      <c r="E92" s="4" t="inlineStr"/>
+      <c r="D92" s="4" t="inlineStr"/>
+      <c r="E92" s="4" t="inlineStr">
+        <is>
+          <t>17:45 - 05:45</t>
+        </is>
+      </c>
       <c r="F92" s="4" t="inlineStr"/>
       <c r="G92" s="4" t="inlineStr"/>
       <c r="H92" s="4" t="inlineStr"/>
@@ -2128,17 +2124,17 @@
     <row r="93">
       <c r="A93" s="4" t="inlineStr">
         <is>
-          <t>Driver_37_12hr</t>
+          <t>Driver_24_12hr</t>
         </is>
       </c>
       <c r="B93" s="4" t="inlineStr"/>
-      <c r="C93" s="4" t="inlineStr"/>
+      <c r="C93" s="4" t="inlineStr">
+        <is>
+          <t>17:45 - 05:45</t>
+        </is>
+      </c>
       <c r="D93" s="4" t="inlineStr"/>
-      <c r="E93" s="4" t="inlineStr">
-        <is>
-          <t>17:45 - 05:45</t>
-        </is>
-      </c>
+      <c r="E93" s="4" t="inlineStr"/>
       <c r="F93" s="4" t="inlineStr"/>
       <c r="G93" s="4" t="inlineStr"/>
       <c r="H93" s="4" t="inlineStr"/>
@@ -2146,7 +2142,7 @@
     <row r="94">
       <c r="A94" s="4" t="inlineStr">
         <is>
-          <t>Driver_40_8hr</t>
+          <t>Driver_26_8hr</t>
         </is>
       </c>
       <c r="B94" s="4" t="inlineStr"/>
@@ -2164,70 +2160,70 @@
     <row r="95">
       <c r="A95" s="4" t="inlineStr">
         <is>
-          <t>Driver_41_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B95" s="4" t="inlineStr"/>
+          <t>Driver_30_12hr</t>
+        </is>
+      </c>
+      <c r="B95" s="4" t="inlineStr">
+        <is>
+          <t>17:45 - 05:45</t>
+        </is>
+      </c>
       <c r="C95" s="4" t="inlineStr"/>
       <c r="D95" s="4" t="inlineStr"/>
       <c r="E95" s="4" t="inlineStr"/>
       <c r="F95" s="4" t="inlineStr"/>
-      <c r="G95" s="4" t="inlineStr">
-        <is>
-          <t>18:48 - 06:48</t>
-        </is>
-      </c>
+      <c r="G95" s="4" t="inlineStr"/>
       <c r="H95" s="4" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="4" t="inlineStr">
         <is>
-          <t>Driver_43_12hr</t>
+          <t>Driver_35_12hr_wk</t>
         </is>
       </c>
       <c r="B96" s="4" t="inlineStr"/>
       <c r="C96" s="4" t="inlineStr"/>
       <c r="D96" s="4" t="inlineStr"/>
       <c r="E96" s="4" t="inlineStr"/>
-      <c r="F96" s="4" t="inlineStr">
-        <is>
-          <t>17:45 - 05:45</t>
-        </is>
-      </c>
+      <c r="F96" s="4" t="inlineStr"/>
       <c r="G96" s="4" t="inlineStr"/>
-      <c r="H96" s="4" t="inlineStr"/>
+      <c r="H96" s="4" t="inlineStr">
+        <is>
+          <t>18:48 - 06:48</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="4" t="inlineStr">
         <is>
-          <t>Driver_44_12hr</t>
+          <t>Driver_47_8hr</t>
         </is>
       </c>
       <c r="B97" s="4" t="inlineStr"/>
       <c r="C97" s="4" t="inlineStr"/>
-      <c r="D97" s="4" t="inlineStr">
-        <is>
-          <t>17:45 - 05:45</t>
-        </is>
-      </c>
+      <c r="D97" s="4" t="inlineStr"/>
       <c r="E97" s="4" t="inlineStr"/>
-      <c r="F97" s="4" t="inlineStr"/>
+      <c r="F97" s="4" t="inlineStr">
+        <is>
+          <t>09:45 - 17:45</t>
+        </is>
+      </c>
       <c r="G97" s="4" t="inlineStr"/>
       <c r="H97" s="4" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="4" t="inlineStr">
         <is>
-          <t>Driver_46_8hr</t>
-        </is>
-      </c>
-      <c r="B98" s="4" t="inlineStr">
-        <is>
-          <t>09:45 - 17:45</t>
-        </is>
-      </c>
+          <t>Driver_52_12hr</t>
+        </is>
+      </c>
+      <c r="B98" s="4" t="inlineStr"/>
       <c r="C98" s="4" t="inlineStr"/>
-      <c r="D98" s="4" t="inlineStr"/>
+      <c r="D98" s="4" t="inlineStr">
+        <is>
+          <t>17:45 - 05:45</t>
+        </is>
+      </c>
       <c r="E98" s="4" t="inlineStr"/>
       <c r="F98" s="4" t="inlineStr"/>
       <c r="G98" s="4" t="inlineStr"/>
@@ -2236,20 +2232,24 @@
     <row r="99">
       <c r="A99" s="4" t="inlineStr">
         <is>
-          <t>Driver_56_12hr_wk</t>
+          <t>Driver_54_8hr</t>
         </is>
       </c>
       <c r="B99" s="4" t="inlineStr"/>
       <c r="C99" s="4" t="inlineStr"/>
-      <c r="D99" s="4" t="inlineStr"/>
-      <c r="E99" s="4" t="inlineStr"/>
+      <c r="D99" s="4" t="inlineStr">
+        <is>
+          <t>09:45 - 17:45</t>
+        </is>
+      </c>
+      <c r="E99" s="4" t="inlineStr">
+        <is>
+          <t>09:45 - 17:45</t>
+        </is>
+      </c>
       <c r="F99" s="4" t="inlineStr"/>
       <c r="G99" s="4" t="inlineStr"/>
-      <c r="H99" s="4" t="inlineStr">
-        <is>
-          <t>18:48 - 06:48</t>
-        </is>
-      </c>
+      <c r="H99" s="4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2262,7 +2262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2342,18 +2342,18 @@
           <t>Driver_4_8hr</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr"/>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>14:15-15:00</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr"/>
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr"/>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr"/>
       <c r="F3" s="4" t="inlineStr"/>
       <c r="G3" s="4" t="inlineStr"/>
       <c r="H3" s="4" t="inlineStr"/>
@@ -2361,7 +2361,7 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>Driver_11_8hr</t>
+          <t>Driver_5_8hr</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
@@ -2369,21 +2369,9 @@
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
+      <c r="C4" s="4" t="inlineStr"/>
+      <c r="D4" s="4" t="inlineStr"/>
+      <c r="E4" s="4" t="inlineStr"/>
       <c r="F4" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
@@ -2395,42 +2383,42 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Driver_12_8hr</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr"/>
+          <t>Driver_11_8hr</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="C5" s="4" t="inlineStr"/>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr"/>
+      <c r="E5" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="F5" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="F5" s="4" t="inlineStr"/>
       <c r="G5" s="4" t="inlineStr"/>
       <c r="H5" s="4" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Driver_18_8hr</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>14:15-15:00</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
+          <t>Driver_12_8hr</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr"/>
+      <c r="C6" s="4" t="inlineStr"/>
+      <c r="D6" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr"/>
       <c r="E6" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
@@ -2443,17 +2431,17 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Driver_19_8hr</t>
+          <t>Driver_18_8hr</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr"/>
       <c r="C7" s="4" t="inlineStr"/>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D7" s="4" t="inlineStr"/>
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr"/>
       <c r="F7" s="4" t="inlineStr"/>
       <c r="G7" s="4" t="inlineStr"/>
       <c r="H7" s="4" t="inlineStr"/>
@@ -2461,56 +2449,60 @@
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Driver_25_8hr</t>
+          <t>Driver_19_8hr</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr"/>
-      <c r="C8" s="4" t="inlineStr"/>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="D8" s="4" t="inlineStr"/>
       <c r="E8" s="4" t="inlineStr"/>
-      <c r="F8" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
+      <c r="F8" s="4" t="inlineStr"/>
       <c r="G8" s="4" t="inlineStr"/>
       <c r="H8" s="4" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Driver_26_8hr</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr"/>
-      <c r="C9" s="4" t="inlineStr"/>
+          <t>Driver_25_8hr</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="D9" s="4" t="inlineStr"/>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
-      <c r="F9" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
+      <c r="E9" s="4" t="inlineStr"/>
+      <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" s="4" t="inlineStr"/>
       <c r="H9" s="4" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>Driver_32_8hr</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr"/>
-      <c r="C10" s="4" t="inlineStr"/>
-      <c r="D10" s="4" t="inlineStr">
+          <t>Driver_26_8hr</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>14:15-15:00</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
+      <c r="D10" s="4" t="inlineStr"/>
       <c r="E10" s="4" t="inlineStr"/>
       <c r="F10" s="4" t="inlineStr"/>
       <c r="G10" s="4" t="inlineStr"/>
@@ -2519,7 +2511,7 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>Driver_33_8hr</t>
+          <t>Driver_32_8hr</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
@@ -2527,28 +2519,36 @@
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr"/>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>14:15-15:00</t>
-        </is>
-      </c>
-      <c r="E11" s="4" t="inlineStr"/>
-      <c r="F11" s="4" t="inlineStr">
-        <is>
           <t>13:00-14:00</t>
         </is>
       </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr"/>
       <c r="G11" s="4" t="inlineStr"/>
       <c r="H11" s="4" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>Driver_39_8hr</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr"/>
+          <t>Driver_33_8hr</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="C12" s="4" t="inlineStr"/>
       <c r="D12" s="4" t="inlineStr">
         <is>
@@ -2563,29 +2563,33 @@
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Driver_40_8hr</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr"/>
+          <t>Driver_39_8hr</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="D13" s="4" t="inlineStr"/>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="E13" s="4" t="inlineStr"/>
-      <c r="F13" s="4" t="inlineStr">
-        <is>
-          <t>14:15-15:00</t>
-        </is>
-      </c>
+      <c r="F13" s="4" t="inlineStr"/>
       <c r="G13" s="4" t="inlineStr"/>
       <c r="H13" s="4" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>Driver_46_8hr</t>
+          <t>Driver_40_8hr</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
@@ -2593,13 +2597,17 @@
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="C14" s="4" t="inlineStr"/>
+      <c r="D14" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="D14" s="4" t="inlineStr"/>
-      <c r="E14" s="4" t="inlineStr"/>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
@@ -2611,47 +2619,39 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Driver_47_8hr</t>
+          <t>Driver_41_12hr_wk</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr"/>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="C15" s="4" t="inlineStr"/>
+      <c r="D15" s="4" t="inlineStr"/>
+      <c r="E15" s="4" t="inlineStr"/>
+      <c r="F15" s="4" t="inlineStr"/>
+      <c r="G15" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="D15" s="4" t="inlineStr"/>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>14:15-15:00</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="inlineStr"/>
-      <c r="G15" s="4" t="inlineStr"/>
       <c r="H15" s="4" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Driver_53_8hr</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
+          <t>Driver_46_8hr</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr"/>
+      <c r="C16" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="D16" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr"/>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
+      <c r="E16" s="4" t="inlineStr"/>
       <c r="F16" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
@@ -2663,73 +2663,85 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Driver_54_8hr</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
+          <t>Driver_47_8hr</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr"/>
+      <c r="C17" s="4" t="inlineStr"/>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>14:15-15:00</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>14:15-15:00</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="F17" s="4" t="inlineStr">
         <is>
           <t>13:00-14:00</t>
         </is>
       </c>
-      <c r="E17" s="4" t="inlineStr"/>
-      <c r="F17" s="4" t="inlineStr"/>
       <c r="G17" s="4" t="inlineStr"/>
       <c r="H17" s="4" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Driver_54_8hr</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr"/>
+      <c r="C18" s="4" t="inlineStr"/>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>14:15-15:00</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr"/>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr"/>
+      <c r="H18" s="4" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>Short Breaks</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr"/>
-      <c r="C18" s="3" t="inlineStr"/>
-      <c r="D18" s="3" t="inlineStr"/>
-      <c r="E18" s="3" t="inlineStr"/>
-      <c r="F18" s="3" t="inlineStr"/>
-      <c r="G18" s="3" t="inlineStr"/>
-      <c r="H18" s="3" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="inlineStr">
-        <is>
-          <t>Driver_1_12hr</t>
-        </is>
-      </c>
-      <c r="B19" s="4" t="inlineStr"/>
-      <c r="C19" s="4" t="inlineStr"/>
-      <c r="D19" s="4" t="inlineStr"/>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
-        </is>
-      </c>
-      <c r="F19" s="4" t="inlineStr"/>
-      <c r="G19" s="4" t="inlineStr"/>
-      <c r="H19" s="4" t="inlineStr"/>
+      <c r="B19" s="3" t="inlineStr"/>
+      <c r="C19" s="3" t="inlineStr"/>
+      <c r="D19" s="3" t="inlineStr"/>
+      <c r="E19" s="3" t="inlineStr"/>
+      <c r="F19" s="3" t="inlineStr"/>
+      <c r="G19" s="3" t="inlineStr"/>
+      <c r="H19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Driver_3_12hr</t>
+          <t>Driver_1_12hr</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr"/>
-      <c r="C20" s="4" t="inlineStr"/>
-      <c r="D20" s="4" t="inlineStr"/>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
+        </is>
+      </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr"/>
@@ -2739,35 +2751,39 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Driver_4_8hr</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="inlineStr"/>
+          <t>Driver_2_12hr</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>16:00-16:18; 18:00-18:18; 20:00-20:18; 22:00-22:18; 00:00-00:18</t>
+        </is>
+      </c>
       <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="4" t="inlineStr"/>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="inlineStr"/>
+      <c r="E21" s="4" t="inlineStr"/>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
+        </is>
+      </c>
       <c r="G21" s="4" t="inlineStr"/>
       <c r="H21" s="4" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Driver_5_8hr</t>
-        </is>
-      </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
-        </is>
-      </c>
+          <t>Driver_3_12hr</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="inlineStr"/>
       <c r="C22" s="4" t="inlineStr"/>
       <c r="D22" s="4" t="inlineStr"/>
-      <c r="E22" s="4" t="inlineStr"/>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
+        </is>
+      </c>
       <c r="F22" s="4" t="inlineStr"/>
       <c r="G22" s="4" t="inlineStr"/>
       <c r="H22" s="4" t="inlineStr"/>
@@ -2775,25 +2791,25 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Driver_6_12hr_wk</t>
+          <t>Driver_5_8hr</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr"/>
-      <c r="C23" s="4" t="inlineStr"/>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
+        </is>
+      </c>
       <c r="D23" s="4" t="inlineStr"/>
       <c r="E23" s="4" t="inlineStr"/>
       <c r="F23" s="4" t="inlineStr"/>
-      <c r="G23" s="4" t="inlineStr">
-        <is>
-          <t>08:00-08:15; 10:00-10:15; 12:00-12:15; 14:00-14:15; 16:00-16:15</t>
-        </is>
-      </c>
+      <c r="G23" s="4" t="inlineStr"/>
       <c r="H23" s="4" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Driver_7_12hr_wk</t>
+          <t>Driver_6_12hr_wk</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr"/>
@@ -2801,12 +2817,12 @@
       <c r="D24" s="4" t="inlineStr"/>
       <c r="E24" s="4" t="inlineStr"/>
       <c r="F24" s="4" t="inlineStr"/>
-      <c r="G24" s="4" t="inlineStr"/>
-      <c r="H24" s="4" t="inlineStr">
-        <is>
-          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
-        </is>
-      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>19:48-20:03; 21:48-22:03; 23:48-00:03; 01:48-02:03; 03:48-04:03</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
@@ -2814,15 +2830,23 @@
           <t>Driver_8_12hr</t>
         </is>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr"/>
+      <c r="C25" s="4" t="inlineStr"/>
+      <c r="D25" s="4" t="inlineStr">
         <is>
           <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
         </is>
       </c>
-      <c r="C25" s="4" t="inlineStr"/>
-      <c r="D25" s="4" t="inlineStr"/>
-      <c r="E25" s="4" t="inlineStr"/>
-      <c r="F25" s="4" t="inlineStr"/>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>16:00-16:18; 18:00-18:18; 20:00-20:18; 22:00-22:18; 00:00-00:18</t>
+        </is>
+      </c>
       <c r="G25" s="4" t="inlineStr"/>
       <c r="H25" s="4" t="inlineStr"/>
     </row>
@@ -2832,15 +2856,23 @@
           <t>Driver_9_12hr</t>
         </is>
       </c>
-      <c r="B26" s="4" t="inlineStr"/>
-      <c r="C26" s="4" t="inlineStr"/>
-      <c r="D26" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="inlineStr">
+        <is>
+          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="inlineStr"/>
       <c r="E26" s="4" t="inlineStr"/>
-      <c r="F26" s="4" t="inlineStr"/>
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
+        </is>
+      </c>
       <c r="G26" s="4" t="inlineStr"/>
       <c r="H26" s="4" t="inlineStr"/>
     </row>
@@ -2856,7 +2888,7 @@
       <c r="E27" s="4" t="inlineStr"/>
       <c r="F27" s="4" t="inlineStr">
         <is>
-          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
+          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
         </is>
       </c>
       <c r="G27" s="4" t="inlineStr"/>
@@ -2894,174 +2926,150 @@
       <c r="G29" s="4" t="inlineStr"/>
       <c r="H29" s="4" t="inlineStr">
         <is>
-          <t>20:33-20:48; 22:33-22:48; 00:33-00:48; 02:33-02:48; 04:33-04:48</t>
+          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Driver_16_12hr</t>
-        </is>
-      </c>
-      <c r="B30" s="4" t="inlineStr">
-        <is>
-          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
-        </is>
-      </c>
+          <t>Driver_15_12hr</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="inlineStr"/>
       <c r="C30" s="4" t="inlineStr"/>
-      <c r="D30" s="4" t="inlineStr"/>
-      <c r="E30" s="4" t="inlineStr">
+      <c r="D30" s="4" t="inlineStr">
         <is>
           <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
         </is>
       </c>
-      <c r="F30" s="4" t="inlineStr">
-        <is>
-          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
-        </is>
-      </c>
+      <c r="E30" s="4" t="inlineStr"/>
+      <c r="F30" s="4" t="inlineStr"/>
       <c r="G30" s="4" t="inlineStr"/>
       <c r="H30" s="4" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Driver_17_12hr</t>
+          <t>Driver_16_12hr</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr"/>
       <c r="C31" s="4" t="inlineStr"/>
-      <c r="D31" s="4" t="inlineStr">
-        <is>
-          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
-        </is>
-      </c>
-      <c r="E31" s="4" t="inlineStr">
-        <is>
-          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
-        </is>
-      </c>
-      <c r="F31" s="4" t="inlineStr"/>
+      <c r="D31" s="4" t="inlineStr"/>
+      <c r="E31" s="4" t="inlineStr"/>
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
+        </is>
+      </c>
       <c r="G31" s="4" t="inlineStr"/>
       <c r="H31" s="4" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Driver_20_12hr_wk</t>
+          <t>Driver_17_12hr</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr"/>
-      <c r="C32" s="4" t="inlineStr"/>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
+        </is>
+      </c>
       <c r="D32" s="4" t="inlineStr"/>
       <c r="E32" s="4" t="inlineStr"/>
       <c r="F32" s="4" t="inlineStr"/>
-      <c r="G32" s="4" t="inlineStr">
-        <is>
-          <t>20:03-20:18; 22:03-22:18; 00:03-00:18; 02:03-02:18; 04:03-04:18</t>
-        </is>
-      </c>
+      <c r="G32" s="4" t="inlineStr"/>
       <c r="H32" s="4" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Driver_23_12hr</t>
-        </is>
-      </c>
-      <c r="B33" s="4" t="inlineStr">
-        <is>
-          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
-        </is>
-      </c>
+          <t>Driver_20_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="inlineStr"/>
       <c r="C33" s="4" t="inlineStr"/>
       <c r="D33" s="4" t="inlineStr"/>
-      <c r="E33" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
+      <c r="E33" s="4" t="inlineStr"/>
       <c r="F33" s="4" t="inlineStr"/>
-      <c r="G33" s="4" t="inlineStr"/>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>20:33-20:48; 22:33-22:48; 00:33-00:48; 02:33-02:48; 04:33-04:48</t>
+        </is>
+      </c>
       <c r="H33" s="4" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Driver_24_12hr</t>
-        </is>
-      </c>
-      <c r="B34" s="4" t="inlineStr">
-        <is>
-          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
-        </is>
-      </c>
-      <c r="C34" s="4" t="inlineStr">
-        <is>
-          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
-        </is>
-      </c>
-      <c r="D34" s="4" t="inlineStr">
-        <is>
-          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
-        </is>
-      </c>
-      <c r="E34" s="4" t="inlineStr">
-        <is>
-          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
-        </is>
-      </c>
+          <t>Driver_21_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B34" s="4" t="inlineStr"/>
+      <c r="C34" s="4" t="inlineStr"/>
+      <c r="D34" s="4" t="inlineStr"/>
+      <c r="E34" s="4" t="inlineStr"/>
       <c r="F34" s="4" t="inlineStr"/>
       <c r="G34" s="4" t="inlineStr"/>
-      <c r="H34" s="4" t="inlineStr"/>
+      <c r="H34" s="4" t="inlineStr">
+        <is>
+          <t>19:48-20:03; 21:48-22:03; 23:48-00:03; 01:48-02:03; 03:48-04:03</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Driver_27_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B35" s="4" t="inlineStr"/>
+          <t>Driver_22_12hr</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
+        </is>
+      </c>
       <c r="C35" s="4" t="inlineStr"/>
       <c r="D35" s="4" t="inlineStr"/>
-      <c r="E35" s="4" t="inlineStr"/>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
+        </is>
+      </c>
       <c r="F35" s="4" t="inlineStr"/>
-      <c r="G35" s="4" t="inlineStr">
-        <is>
-          <t>08:15-08:30; 10:15-10:30; 12:15-12:30; 14:15-14:30; 16:15-16:30</t>
-        </is>
-      </c>
+      <c r="G35" s="4" t="inlineStr"/>
       <c r="H35" s="4" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Driver_28_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B36" s="4" t="inlineStr"/>
+          <t>Driver_23_12hr</t>
+        </is>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
       <c r="C36" s="4" t="inlineStr"/>
       <c r="D36" s="4" t="inlineStr"/>
       <c r="E36" s="4" t="inlineStr"/>
       <c r="F36" s="4" t="inlineStr"/>
       <c r="G36" s="4" t="inlineStr"/>
-      <c r="H36" s="4" t="inlineStr">
-        <is>
-          <t>08:30-08:45; 10:30-10:45; 12:30-12:45; 14:30-14:45; 16:30-16:45</t>
-        </is>
-      </c>
+      <c r="H36" s="4" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Driver_29_12hr</t>
+          <t>Driver_24_12hr</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr"/>
       <c r="C37" s="4" t="inlineStr">
         <is>
-          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
+          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
         </is>
       </c>
       <c r="D37" s="4" t="inlineStr"/>
@@ -3073,65 +3081,53 @@
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Driver_30_12hr</t>
-        </is>
-      </c>
-      <c r="B38" s="4" t="inlineStr">
-        <is>
-          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
-        </is>
-      </c>
+          <t>Driver_27_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B38" s="4" t="inlineStr"/>
       <c r="C38" s="4" t="inlineStr"/>
       <c r="D38" s="4" t="inlineStr"/>
       <c r="E38" s="4" t="inlineStr"/>
       <c r="F38" s="4" t="inlineStr"/>
-      <c r="G38" s="4" t="inlineStr"/>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
+        </is>
+      </c>
       <c r="H38" s="4" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Driver_31_12hr</t>
+          <t>Driver_28_12hr_wk</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr"/>
-      <c r="C39" s="4" t="inlineStr">
-        <is>
-          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
-        </is>
-      </c>
+      <c r="C39" s="4" t="inlineStr"/>
       <c r="D39" s="4" t="inlineStr"/>
-      <c r="E39" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
-      <c r="F39" s="4" t="inlineStr">
-        <is>
-          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
-        </is>
-      </c>
+      <c r="E39" s="4" t="inlineStr"/>
+      <c r="F39" s="4" t="inlineStr"/>
       <c r="G39" s="4" t="inlineStr"/>
-      <c r="H39" s="4" t="inlineStr"/>
+      <c r="H39" s="4" t="inlineStr">
+        <is>
+          <t>20:33-20:48; 22:33-22:48; 00:33-00:48; 02:33-02:48; 04:33-04:48</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Driver_33_8hr</t>
+          <t>Driver_29_12hr</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr"/>
       <c r="C40" s="4" t="inlineStr">
         <is>
-          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
+          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
         </is>
       </c>
       <c r="D40" s="4" t="inlineStr"/>
-      <c r="E40" s="4" t="inlineStr">
-        <is>
-          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
-        </is>
-      </c>
+      <c r="E40" s="4" t="inlineStr"/>
       <c r="F40" s="4" t="inlineStr"/>
       <c r="G40" s="4" t="inlineStr"/>
       <c r="H40" s="4" t="inlineStr"/>
@@ -3139,108 +3135,96 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Driver_34_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B41" s="4" t="inlineStr"/>
+          <t>Driver_30_12hr</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
+        </is>
+      </c>
       <c r="C41" s="4" t="inlineStr"/>
-      <c r="D41" s="4" t="inlineStr"/>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
+        </is>
+      </c>
       <c r="E41" s="4" t="inlineStr"/>
       <c r="F41" s="4" t="inlineStr"/>
-      <c r="G41" s="4" t="inlineStr">
-        <is>
-          <t>08:30-08:45; 10:30-10:45; 12:30-12:45; 14:30-14:45; 16:30-16:45</t>
-        </is>
-      </c>
+      <c r="G41" s="4" t="inlineStr"/>
       <c r="H41" s="4" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Driver_35_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B42" s="4" t="inlineStr"/>
+          <t>Driver_31_12hr</t>
+        </is>
+      </c>
+      <c r="B42" s="4" t="inlineStr">
+        <is>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
+        </is>
+      </c>
       <c r="C42" s="4" t="inlineStr"/>
       <c r="D42" s="4" t="inlineStr"/>
       <c r="E42" s="4" t="inlineStr"/>
       <c r="F42" s="4" t="inlineStr"/>
       <c r="G42" s="4" t="inlineStr"/>
-      <c r="H42" s="4" t="inlineStr">
-        <is>
-          <t>08:15-08:30; 10:15-10:30; 12:15-12:30; 14:15-14:30; 16:15-16:30</t>
-        </is>
-      </c>
+      <c r="H42" s="4" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Driver_36_12hr</t>
+          <t>Driver_34_12hr_wk</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr"/>
-      <c r="C43" s="4" t="inlineStr">
-        <is>
-          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
-        </is>
-      </c>
-      <c r="D43" s="4" t="inlineStr">
-        <is>
-          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
-        </is>
-      </c>
+      <c r="C43" s="4" t="inlineStr"/>
+      <c r="D43" s="4" t="inlineStr"/>
       <c r="E43" s="4" t="inlineStr"/>
-      <c r="F43" s="4" t="inlineStr">
-        <is>
-          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
-        </is>
-      </c>
-      <c r="G43" s="4" t="inlineStr"/>
+      <c r="F43" s="4" t="inlineStr"/>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>08:00-08:15; 10:00-10:15; 12:00-12:15; 14:00-14:15; 16:00-16:15</t>
+        </is>
+      </c>
       <c r="H43" s="4" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Driver_37_12hr</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
+          <t>Driver_35_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="inlineStr"/>
       <c r="C44" s="4" t="inlineStr"/>
-      <c r="D44" s="4" t="inlineStr">
-        <is>
-          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
-        </is>
-      </c>
-      <c r="E44" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
+      <c r="D44" s="4" t="inlineStr"/>
+      <c r="E44" s="4" t="inlineStr"/>
       <c r="F44" s="4" t="inlineStr"/>
       <c r="G44" s="4" t="inlineStr"/>
-      <c r="H44" s="4" t="inlineStr"/>
+      <c r="H44" s="4" t="inlineStr">
+        <is>
+          <t>08:30-08:45; 10:30-10:45; 12:30-12:45; 14:30-14:45; 16:30-16:45</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Driver_38_12hr</t>
+          <t>Driver_36_12hr</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr"/>
       <c r="C45" s="4" t="inlineStr"/>
-      <c r="D45" s="4" t="inlineStr">
-        <is>
-          <t>16:00-16:18; 18:00-18:18; 20:00-20:18; 22:00-22:18; 00:00-00:18</t>
-        </is>
-      </c>
-      <c r="E45" s="4" t="inlineStr"/>
+      <c r="D45" s="4" t="inlineStr"/>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
       <c r="F45" s="4" t="inlineStr">
         <is>
-          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
+          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
         </is>
       </c>
       <c r="G45" s="4" t="inlineStr"/>
@@ -3249,56 +3233,56 @@
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Driver_41_12hr_wk</t>
-        </is>
-      </c>
-      <c r="B46" s="4" t="inlineStr"/>
+          <t>Driver_37_12hr</t>
+        </is>
+      </c>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
+        </is>
+      </c>
       <c r="C46" s="4" t="inlineStr"/>
-      <c r="D46" s="4" t="inlineStr"/>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
       <c r="E46" s="4" t="inlineStr"/>
       <c r="F46" s="4" t="inlineStr"/>
-      <c r="G46" s="4" t="inlineStr">
-        <is>
-          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
-        </is>
-      </c>
+      <c r="G46" s="4" t="inlineStr"/>
       <c r="H46" s="4" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Driver_42_12hr_wk</t>
+          <t>Driver_38_12hr</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr"/>
       <c r="C47" s="4" t="inlineStr"/>
       <c r="D47" s="4" t="inlineStr"/>
       <c r="E47" s="4" t="inlineStr"/>
-      <c r="F47" s="4" t="inlineStr"/>
+      <c r="F47" s="4" t="inlineStr">
+        <is>
+          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
+        </is>
+      </c>
       <c r="G47" s="4" t="inlineStr"/>
-      <c r="H47" s="4" t="inlineStr">
-        <is>
-          <t>08:00-08:15; 10:00-10:15; 12:00-12:15; 14:00-14:15; 16:00-16:15</t>
-        </is>
-      </c>
+      <c r="H47" s="4" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Driver_43_12hr</t>
-        </is>
-      </c>
-      <c r="B48" s="4" t="inlineStr">
-        <is>
-          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
-        </is>
-      </c>
+          <t>Driver_39_8hr</t>
+        </is>
+      </c>
+      <c r="B48" s="4" t="inlineStr"/>
       <c r="C48" s="4" t="inlineStr"/>
       <c r="D48" s="4" t="inlineStr"/>
       <c r="E48" s="4" t="inlineStr"/>
       <c r="F48" s="4" t="inlineStr">
         <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
+          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
         </is>
       </c>
       <c r="G48" s="4" t="inlineStr"/>
@@ -3307,47 +3291,43 @@
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Driver_44_12hr</t>
+          <t>Driver_42_12hr_wk</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr"/>
-      <c r="C49" s="4" t="inlineStr">
-        <is>
-          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
-        </is>
-      </c>
-      <c r="D49" s="4" t="inlineStr">
-        <is>
-          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
-        </is>
-      </c>
+      <c r="C49" s="4" t="inlineStr"/>
+      <c r="D49" s="4" t="inlineStr"/>
       <c r="E49" s="4" t="inlineStr"/>
-      <c r="F49" s="4" t="inlineStr">
-        <is>
-          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
-        </is>
-      </c>
+      <c r="F49" s="4" t="inlineStr"/>
       <c r="G49" s="4" t="inlineStr"/>
-      <c r="H49" s="4" t="inlineStr"/>
+      <c r="H49" s="4" t="inlineStr">
+        <is>
+          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Driver_45_12hr</t>
+          <t>Driver_43_12hr</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr"/>
       <c r="C50" s="4" t="inlineStr">
         <is>
-          <t>18:45-19:03; 20:45-21:03; 22:45-23:03; 00:45-01:03; 02:45-03:03</t>
+          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
         </is>
       </c>
       <c r="D50" s="4" t="inlineStr">
         <is>
-          <t>16:00-16:18; 18:00-18:18; 20:00-20:18; 22:00-22:18; 00:00-00:18</t>
-        </is>
-      </c>
-      <c r="E50" s="4" t="inlineStr"/>
+          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
       <c r="F50" s="4" t="inlineStr"/>
       <c r="G50" s="4" t="inlineStr"/>
       <c r="H50" s="4" t="inlineStr"/>
@@ -3355,25 +3335,29 @@
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Driver_47_8hr</t>
-        </is>
-      </c>
-      <c r="B51" s="4" t="inlineStr"/>
-      <c r="C51" s="4" t="inlineStr"/>
+          <t>Driver_44_12hr</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
+        </is>
+      </c>
       <c r="D51" s="4" t="inlineStr"/>
       <c r="E51" s="4" t="inlineStr"/>
-      <c r="F51" s="4" t="inlineStr">
-        <is>
-          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
-        </is>
-      </c>
+      <c r="F51" s="4" t="inlineStr"/>
       <c r="G51" s="4" t="inlineStr"/>
       <c r="H51" s="4" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Driver_48_12hr_wk</t>
+          <t>Driver_49_12hr_wk</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr"/>
@@ -3381,12 +3365,12 @@
       <c r="D52" s="4" t="inlineStr"/>
       <c r="E52" s="4" t="inlineStr"/>
       <c r="F52" s="4" t="inlineStr"/>
-      <c r="G52" s="4" t="inlineStr">
+      <c r="G52" s="4" t="inlineStr"/>
+      <c r="H52" s="4" t="inlineStr">
         <is>
           <t>20:33-20:48; 22:33-22:48; 00:33-00:48; 02:33-02:48; 04:33-04:48</t>
         </is>
       </c>
-      <c r="H52" s="4" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
@@ -3397,7 +3381,7 @@
       <c r="B53" s="4" t="inlineStr"/>
       <c r="C53" s="4" t="inlineStr">
         <is>
-          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
+          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
         </is>
       </c>
       <c r="D53" s="4" t="inlineStr"/>
@@ -3412,59 +3396,117 @@
           <t>Driver_51_12hr</t>
         </is>
       </c>
-      <c r="B54" s="4" t="inlineStr">
-        <is>
-          <t>16:30-16:48; 18:30-18:48; 20:30-20:48; 22:30-22:48; 00:30-00:48</t>
-        </is>
-      </c>
-      <c r="C54" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
-      <c r="D54" s="4" t="inlineStr"/>
-      <c r="E54" s="4" t="inlineStr"/>
-      <c r="F54" s="4" t="inlineStr">
-        <is>
-          <t>19:00-19:18; 21:00-21:18; 23:00-23:18; 01:00-01:18; 03:00-03:18</t>
-        </is>
-      </c>
+      <c r="B54" s="4" t="inlineStr"/>
+      <c r="C54" s="4" t="inlineStr"/>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>19:30-19:48; 21:30-21:48; 23:30-23:48; 01:30-01:48; 03:30-03:48</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>15:45-16:03; 17:45-18:03; 19:45-20:03; 21:45-22:03; 23:45-00:03</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr"/>
       <c r="G54" s="4" t="inlineStr"/>
       <c r="H54" s="4" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Driver_55_12hr_wk</t>
+          <t>Driver_52_12hr</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr"/>
       <c r="C55" s="4" t="inlineStr"/>
-      <c r="D55" s="4" t="inlineStr"/>
-      <c r="E55" s="4" t="inlineStr"/>
-      <c r="F55" s="4" t="inlineStr"/>
-      <c r="G55" s="4" t="inlineStr">
-        <is>
-          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
-        </is>
-      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>16:15-16:33; 18:15-18:33; 20:15-20:33; 22:15-22:33; 00:15-00:33</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
+        </is>
+      </c>
+      <c r="F55" s="4" t="inlineStr">
+        <is>
+          <t>19:15-19:33; 21:15-21:33; 23:15-23:33; 01:15-01:33; 03:15-03:33</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr"/>
       <c r="H55" s="4" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>Driver_56_12hr_wk</t>
+          <t>Driver_53_8hr</t>
         </is>
       </c>
       <c r="B56" s="4" t="inlineStr"/>
       <c r="C56" s="4" t="inlineStr"/>
       <c r="D56" s="4" t="inlineStr"/>
       <c r="E56" s="4" t="inlineStr"/>
-      <c r="F56" s="4" t="inlineStr"/>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
+        </is>
+      </c>
       <c r="G56" s="4" t="inlineStr"/>
-      <c r="H56" s="4" t="inlineStr">
-        <is>
-          <t>19:48-20:03; 21:48-22:03; 23:48-00:03; 01:48-02:03; 03:48-04:03</t>
+      <c r="H56" s="4" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="inlineStr">
+        <is>
+          <t>Driver_54_8hr</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="inlineStr"/>
+      <c r="C57" s="4" t="inlineStr"/>
+      <c r="D57" s="4" t="inlineStr"/>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>07:45-08:00; 09:45-10:00; 11:45-12:00</t>
+        </is>
+      </c>
+      <c r="F57" s="4" t="inlineStr"/>
+      <c r="G57" s="4" t="inlineStr"/>
+      <c r="H57" s="4" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>Driver_55_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B58" s="4" t="inlineStr"/>
+      <c r="C58" s="4" t="inlineStr"/>
+      <c r="D58" s="4" t="inlineStr"/>
+      <c r="E58" s="4" t="inlineStr"/>
+      <c r="F58" s="4" t="inlineStr"/>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>20:18-20:33; 22:18-22:33; 00:18-00:33; 02:18-02:33; 04:18-04:33</t>
+        </is>
+      </c>
+      <c r="H58" s="4" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="inlineStr">
+        <is>
+          <t>Driver_56_12hr_wk</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="inlineStr"/>
+      <c r="C59" s="4" t="inlineStr"/>
+      <c r="D59" s="4" t="inlineStr"/>
+      <c r="E59" s="4" t="inlineStr"/>
+      <c r="F59" s="4" t="inlineStr"/>
+      <c r="G59" s="4" t="inlineStr"/>
+      <c r="H59" s="4" t="inlineStr">
+        <is>
+          <t>20:03-20:18; 22:03-22:18; 00:03-00:18; 02:03-02:18; 04:03-04:18</t>
         </is>
       </c>
     </row>

</xml_diff>